<commit_message>
send df to Visu tab new
</commit_message>
<xml_diff>
--- a/data_test/df4.xlsx
+++ b/data_test/df4.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HoanLe/SPECTROview/Python/data_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7400A32C-543C-0340-A00A-2FE45661B811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73393E04-1A0F-DE44-82E2-6D93B9FAE34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SiGe20" sheetId="1" r:id="rId1"/>
+    <sheet name="SiGe30" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="53">
   <si>
     <t>zone</t>
   </si>
@@ -695,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1812,869 +1813,919 @@
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="5">
-        <v>30</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H35" s="6">
-        <v>520.76599999999996</v>
-      </c>
-      <c r="I35" s="6">
-        <v>3.5810200000000001</v>
-      </c>
-      <c r="J35" s="6">
-        <v>512.28199999999993</v>
-      </c>
-      <c r="K35" s="6">
-        <v>12.199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="5">
-        <v>30</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="6">
-        <v>520.78800000000001</v>
-      </c>
-      <c r="I36" s="6">
-        <v>3.6238700000000001</v>
-      </c>
-      <c r="J36" s="6">
-        <v>511.39699999999999</v>
-      </c>
-      <c r="K36" s="6">
-        <v>14.6768</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="14">
-        <v>30</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="16">
-        <v>520.79599999999994</v>
-      </c>
-      <c r="I37" s="16">
-        <v>3.5990500000000001</v>
-      </c>
-      <c r="J37" s="16">
-        <v>512.37699999999995</v>
-      </c>
-      <c r="K37" s="16">
-        <v>11.384499999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="7">
-        <v>30</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H38" s="8">
-        <v>517.57249999999988</v>
-      </c>
-      <c r="I38" s="8">
-        <v>4.5979400000000004</v>
-      </c>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="7">
-        <v>30</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H39" s="8">
-        <v>517.72449999999992</v>
-      </c>
-      <c r="I39" s="8">
-        <v>4.4561299999999999</v>
-      </c>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="7">
-        <v>30</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H40" s="8">
-        <v>517.80749999999989</v>
-      </c>
-      <c r="I40" s="8">
-        <v>4.4601199999999999</v>
-      </c>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="7">
-        <v>30</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H41" s="8">
-        <v>517.77949999999998</v>
-      </c>
-      <c r="I41" s="8">
-        <v>4.40822</v>
-      </c>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="10">
-        <v>30</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G42" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H42" s="11">
-        <v>517.78849999999989</v>
-      </c>
-      <c r="I42" s="11">
-        <v>4.4452100000000003</v>
-      </c>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="7">
-        <v>30</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H43" s="8">
-        <v>517.51349999999991</v>
-      </c>
-      <c r="I43" s="8">
-        <v>4.7114399999999996</v>
-      </c>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="7">
-        <v>30</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H44" s="8">
-        <v>517.64649999999995</v>
-      </c>
-      <c r="I44" s="8">
-        <v>4.4549899999999996</v>
-      </c>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="7">
-        <v>30</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H45" s="8">
-        <v>517.7645</v>
-      </c>
-      <c r="I45" s="8">
-        <v>4.3731499999999999</v>
-      </c>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="7">
-        <v>30</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H46" s="8">
-        <v>517.6434999999999</v>
-      </c>
-      <c r="I46" s="8">
-        <v>4.47227</v>
-      </c>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="10">
-        <v>30</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G47" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="11">
-        <v>517.72149999999999</v>
-      </c>
-      <c r="I47" s="11">
-        <v>4.3412899999999999</v>
-      </c>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="7">
-        <v>30</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G48" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H48" s="8">
-        <v>520.66649999999993</v>
-      </c>
-      <c r="I48" s="8">
-        <v>4.0194700000000001</v>
-      </c>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="7">
-        <v>30</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H49" s="8">
-        <v>520.64</v>
-      </c>
-      <c r="I49" s="8">
-        <v>3.8713099999999998</v>
-      </c>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="10">
-        <v>30</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G50" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="H50" s="11">
-        <v>520.53599999999994</v>
-      </c>
-      <c r="I50" s="11">
-        <v>4.1363000000000003</v>
-      </c>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="7">
-        <v>30</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H51" s="8">
-        <v>518.62299999999993</v>
-      </c>
-      <c r="I51" s="8">
-        <v>4.2135199999999999</v>
-      </c>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="7">
-        <v>30</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G52" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H52" s="8">
-        <v>518.61599999999999</v>
-      </c>
-      <c r="I52" s="8">
-        <v>4.2448800000000002</v>
-      </c>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="10">
-        <v>30</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H53" s="11">
-        <v>518.44099999999992</v>
-      </c>
-      <c r="I53" s="11">
-        <v>4.4798799999999996</v>
-      </c>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="30">
-        <v>30</v>
-      </c>
-      <c r="F54" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="G54" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H54" s="32">
-        <v>517.77649999999994</v>
-      </c>
-      <c r="I54" s="32">
-        <v>4.4058099999999998</v>
-      </c>
-      <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="7">
-        <v>30</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="8">
-        <v>518.86549999999988</v>
-      </c>
-      <c r="I55" s="8">
-        <v>4.6873199999999997</v>
-      </c>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E56" s="10">
-        <v>30</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G56" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H56" s="11">
-        <v>518.96549999999991</v>
-      </c>
-      <c r="I56" s="11">
-        <v>4.5316000000000001</v>
-      </c>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E57" s="7">
-        <v>30</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G57" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H57" s="8">
-        <v>518.82749999999999</v>
-      </c>
-      <c r="I57" s="8">
-        <v>4.4201499999999996</v>
-      </c>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E58" s="10">
-        <v>30</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G58" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H58" s="11">
-        <v>518.78849999999989</v>
-      </c>
-      <c r="I58" s="11">
-        <v>4.4696600000000002</v>
-      </c>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E59" s="5">
-        <v>30</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H59" s="6">
-        <v>519.7505000000001</v>
-      </c>
-      <c r="I59" s="6">
-        <v>3.6774399999999998</v>
-      </c>
-      <c r="J59" s="6">
-        <v>510.32650000000007</v>
-      </c>
-      <c r="K59" s="6">
-        <v>17.072500000000002</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="5">
-        <v>30</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H60" s="6">
-        <v>520.82650000000001</v>
-      </c>
-      <c r="I60" s="6">
-        <v>3.5160300000000002</v>
-      </c>
-      <c r="J60" s="6">
-        <v>511.22550000000007</v>
-      </c>
-      <c r="K60" s="6">
-        <v>15.021599999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" s="5">
-        <v>30</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H61" s="6">
-        <v>520.678</v>
-      </c>
-      <c r="I61" s="6">
-        <v>3.6620200000000001</v>
-      </c>
-      <c r="J61" s="6">
-        <v>510.46700000000004</v>
-      </c>
-      <c r="K61" s="6">
-        <v>14.818899999999999</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA2C61B-DD48-A648-B81D-780CD76772B9}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5">
+        <v>30</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="6">
+        <v>520.76599999999996</v>
+      </c>
+      <c r="I2" s="6">
+        <v>3.5810200000000001</v>
+      </c>
+      <c r="J2" s="6">
+        <v>512.28199999999993</v>
+      </c>
+      <c r="K2" s="6">
+        <v>12.199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="6">
+        <v>520.78800000000001</v>
+      </c>
+      <c r="I3" s="6">
+        <v>3.6238700000000001</v>
+      </c>
+      <c r="J3" s="6">
+        <v>511.39699999999999</v>
+      </c>
+      <c r="K3" s="6">
+        <v>14.6768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="14">
+        <v>30</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="16">
+        <v>520.79599999999994</v>
+      </c>
+      <c r="I4" s="16">
+        <v>3.5990500000000001</v>
+      </c>
+      <c r="J4" s="16">
+        <v>512.37699999999995</v>
+      </c>
+      <c r="K4" s="16">
+        <v>11.384499999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7">
+        <v>30</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="8">
+        <v>517.57249999999988</v>
+      </c>
+      <c r="I5" s="8">
+        <v>4.5979400000000004</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="7">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="8">
+        <v>517.72449999999992</v>
+      </c>
+      <c r="I6" s="8">
+        <v>4.4561299999999999</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="8">
+        <v>517.80749999999989</v>
+      </c>
+      <c r="I7" s="8">
+        <v>4.4601199999999999</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7">
+        <v>30</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="8">
+        <v>517.77949999999998</v>
+      </c>
+      <c r="I8" s="8">
+        <v>4.40822</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="10">
+        <v>30</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="11">
+        <v>517.78849999999989</v>
+      </c>
+      <c r="I9" s="11">
+        <v>4.4452100000000003</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7">
+        <v>30</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="8">
+        <v>517.51349999999991</v>
+      </c>
+      <c r="I10" s="8">
+        <v>4.7114399999999996</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="7">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="8">
+        <v>517.64649999999995</v>
+      </c>
+      <c r="I11" s="8">
+        <v>4.4549899999999996</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="7">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="8">
+        <v>517.7645</v>
+      </c>
+      <c r="I12" s="8">
+        <v>4.3731499999999999</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="7">
+        <v>30</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="8">
+        <v>517.6434999999999</v>
+      </c>
+      <c r="I13" s="8">
+        <v>4.47227</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="10">
+        <v>30</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="11">
+        <v>517.72149999999999</v>
+      </c>
+      <c r="I14" s="11">
+        <v>4.3412899999999999</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="7">
+        <v>30</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="8">
+        <v>520.66649999999993</v>
+      </c>
+      <c r="I15" s="8">
+        <v>4.0194700000000001</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="7">
+        <v>30</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="8">
+        <v>520.64</v>
+      </c>
+      <c r="I16" s="8">
+        <v>3.8713099999999998</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="10">
+        <v>30</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="11">
+        <v>520.53599999999994</v>
+      </c>
+      <c r="I17" s="11">
+        <v>4.1363000000000003</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="7">
+        <v>30</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="8">
+        <v>518.62299999999993</v>
+      </c>
+      <c r="I18" s="8">
+        <v>4.2135199999999999</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="7">
+        <v>30</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="8">
+        <v>518.61599999999999</v>
+      </c>
+      <c r="I19" s="8">
+        <v>4.2448800000000002</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="10">
+        <v>30</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="11">
+        <v>518.44099999999992</v>
+      </c>
+      <c r="I20" s="11">
+        <v>4.4798799999999996</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="30">
+        <v>30</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="32">
+        <v>517.77649999999994</v>
+      </c>
+      <c r="I21" s="32">
+        <v>4.4058099999999998</v>
+      </c>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="7">
+        <v>30</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="8">
+        <v>518.86549999999988</v>
+      </c>
+      <c r="I22" s="8">
+        <v>4.6873199999999997</v>
+      </c>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="10">
+        <v>30</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="11">
+        <v>518.96549999999991</v>
+      </c>
+      <c r="I23" s="11">
+        <v>4.5316000000000001</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="7">
+        <v>30</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="8">
+        <v>518.82749999999999</v>
+      </c>
+      <c r="I24" s="8">
+        <v>4.4201499999999996</v>
+      </c>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="10">
+        <v>30</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="11">
+        <v>518.78849999999989</v>
+      </c>
+      <c r="I25" s="11">
+        <v>4.4696600000000002</v>
+      </c>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="5">
+        <v>30</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="6">
+        <v>519.7505000000001</v>
+      </c>
+      <c r="I26" s="6">
+        <v>3.6774399999999998</v>
+      </c>
+      <c r="J26" s="6">
+        <v>510.32650000000007</v>
+      </c>
+      <c r="K26" s="6">
+        <v>17.072500000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="5">
+        <v>30</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="6">
+        <v>520.82650000000001</v>
+      </c>
+      <c r="I27" s="6">
+        <v>3.5160300000000002</v>
+      </c>
+      <c r="J27" s="6">
+        <v>511.22550000000007</v>
+      </c>
+      <c r="K27" s="6">
+        <v>15.021599999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="5">
+        <v>30</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="6">
+        <v>520.678</v>
+      </c>
+      <c r="I28" s="6">
+        <v>3.6620200000000001</v>
+      </c>
+      <c r="J28" s="6">
+        <v>510.46700000000004</v>
+      </c>
+      <c r="K28" s="6">
+        <v>14.818899999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>